<commit_message>
cambios analisis tiempo req 2 y 4
</commit_message>
<xml_diff>
--- a/Docs/Tiempos 1,2,3,4,5.xlsx
+++ b/Docs/Tiempos 1,2,3,4,5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jgril\Desktop\programar\proyectos\Reto3-05\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77225EE3-F8E4-4C1E-82E9-0DE314D5E706}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{152D23AE-3477-4522-BEB9-98707B4D23D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4515" yWindow="6735" windowWidth="21315" windowHeight="8055" xr2:uid="{D82936D8-D2C9-4EB2-9CBC-3665F65B95FD}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="26">
   <si>
     <t>Porcentaje de la muestra [pct]</t>
   </si>
@@ -77,10 +77,52 @@
     <t>Requerimiento 5 [ms]</t>
   </si>
   <si>
-    <t>Requerimiento 2</t>
+    <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>Requerimiento 4</t>
+    <t>Columna1</t>
+  </si>
+  <si>
+    <t>REQUERIMIENTO 2</t>
+  </si>
+  <si>
+    <t>REQUERIMIENTO 4</t>
+  </si>
+  <si>
+    <t>Small:</t>
+  </si>
+  <si>
+    <t>10pct:</t>
+  </si>
+  <si>
+    <t>50pct:</t>
+  </si>
+  <si>
+    <t>large:</t>
+  </si>
+  <si>
+    <t>4.96ms</t>
+  </si>
+  <si>
+    <t>10.3ms</t>
+  </si>
+  <si>
+    <t>30.44ms</t>
+  </si>
+  <si>
+    <t>40.52ms</t>
+  </si>
+  <si>
+    <t>6.00ms</t>
+  </si>
+  <si>
+    <t>15.647ms</t>
+  </si>
+  <si>
+    <t>43.678ms</t>
+  </si>
+  <si>
+    <t>90,68ms</t>
   </si>
 </sst>
 </file>
@@ -2219,6 +2261,18 @@
                     <c:numCache>
                       <c:formatCode>0.00</c:formatCode>
                       <c:ptCount val="8"/>
+                      <c:pt idx="2">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>0</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:yVal>
@@ -4361,8 +4415,8 @@
     <tableColumn id="3" xr3:uid="{19B1D273-887B-4392-991E-015D36D99E5B}" name="Requerimiento 1 [ms]" dataDxfId="4"/>
     <tableColumn id="4" xr3:uid="{56471E76-DCC6-4EED-8237-BCC256B57E91}" name="Requerimiento 3 [ms]" dataDxfId="3"/>
     <tableColumn id="5" xr3:uid="{61DF25D7-A2A3-4D39-B0C6-29804C1B33DB}" name="Requerimiento 5 [ms]" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{6FC8F4B7-6274-4B14-98D8-0E00E479351A}" name="Requerimiento 2" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{5EBC2ECC-1A75-4BE6-ACD3-41C97731C087}" name="Requerimiento 4" dataDxfId="0"/>
+    <tableColumn id="6" xr3:uid="{6FC8F4B7-6274-4B14-98D8-0E00E479351A}" name="Columna1" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{5EBC2ECC-1A75-4BE6-ACD3-41C97731C087}" name=" " dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4667,8 +4721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5B14742-4EBB-4241-AC8A-0E5F24F7BB7B}">
   <dimension ref="A1:M83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -4678,8 +4732,8 @@
     <col min="3" max="3" width="21.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.140625" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" customWidth="1"/>
+    <col min="7" max="7" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="8" customFormat="1" ht="30">
@@ -4699,10 +4753,10 @@
         <v>9</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="6" t="s">
         <v>10</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>11</v>
       </c>
       <c r="I1" s="10"/>
       <c r="J1" s="10"/>
@@ -4921,7 +4975,7 @@
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:13" ht="28.5">
       <c r="A14" s="5" t="s">
         <v>5</v>
       </c>
@@ -4935,8 +4989,12 @@
         <v>15.625</v>
       </c>
       <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
+      <c r="F14" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>13</v>
+      </c>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
     </row>
@@ -4953,9 +5011,15 @@
       <c r="D15" s="3">
         <v>15.625</v>
       </c>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
+      <c r="E15" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
     </row>
@@ -4972,24 +5036,45 @@
       <c r="D16" s="3">
         <v>15.625</v>
       </c>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
+      <c r="E16" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G16" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="5"/>
       <c r="B17" s="7"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
+      <c r="E17" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G17" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="5"/>
       <c r="B18" s="7"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
+      <c r="E18" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G18" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="5">
@@ -5389,112 +5474,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="85e30bcc-d76c-4413-8e4d-2dce22fb0743">
-      <UserInfo>
-        <DisplayName>Carlos Andres Lozano Garzon</DisplayName>
-        <AccountId>13</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Dario Ernesto Correal Torres</DisplayName>
-        <AccountId>15</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Mario  Fernando De la rosa Rosero</DisplayName>
-        <AccountId>16</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Christian Camilo Aparicio Baquen</DisplayName>
-        <AccountId>50</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Arturo Henao Chaparro</DisplayName>
-        <AccountId>48</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Luis Esteban Florez Salamanca</DisplayName>
-        <AccountId>33</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Ivan David Salazar Cardenas</DisplayName>
-        <AccountId>52</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Juan Carlos Marin Morales</DisplayName>
-        <AccountId>53</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Sofia Duque Gomez</DisplayName>
-        <AccountId>60</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Andres Felipe Romero Brand</DisplayName>
-        <AccountId>91</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Lindsay Vanessa Pinto Morato</DisplayName>
-        <AccountId>92</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Miguel Angel Acosta Walteros</DisplayName>
-        <AccountId>94</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Juan David Diaz Ipuz</DisplayName>
-        <AccountId>90</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Lily Aitana valentina Duque Chavez</DisplayName>
-        <AccountId>17</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Isaac David Bermudez Lara</DisplayName>
-        <AccountId>95</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Daniel Alejandro Angel Fuertes</DisplayName>
-        <AccountId>55</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Jeniffer Liliam Mendoza Espinosa</DisplayName>
-        <AccountId>97</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Kevin Cohen Solano</DisplayName>
-        <AccountId>93</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Cesar Luis Moreno Gonzalez</DisplayName>
-        <AccountId>96</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Jose Cristobal Arroyo Castellanos</DisplayName>
-        <AccountId>54</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5715,27 +5700,118 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="85e30bcc-d76c-4413-8e4d-2dce22fb0743">
+      <UserInfo>
+        <DisplayName>Carlos Andres Lozano Garzon</DisplayName>
+        <AccountId>13</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Dario Ernesto Correal Torres</DisplayName>
+        <AccountId>15</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Mario  Fernando De la rosa Rosero</DisplayName>
+        <AccountId>16</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Christian Camilo Aparicio Baquen</DisplayName>
+        <AccountId>50</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Arturo Henao Chaparro</DisplayName>
+        <AccountId>48</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Luis Esteban Florez Salamanca</DisplayName>
+        <AccountId>33</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Ivan David Salazar Cardenas</DisplayName>
+        <AccountId>52</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Juan Carlos Marin Morales</DisplayName>
+        <AccountId>53</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Sofia Duque Gomez</DisplayName>
+        <AccountId>60</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Andres Felipe Romero Brand</DisplayName>
+        <AccountId>91</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Lindsay Vanessa Pinto Morato</DisplayName>
+        <AccountId>92</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Miguel Angel Acosta Walteros</DisplayName>
+        <AccountId>94</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Juan David Diaz Ipuz</DisplayName>
+        <AccountId>90</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Lily Aitana valentina Duque Chavez</DisplayName>
+        <AccountId>17</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Isaac David Bermudez Lara</DisplayName>
+        <AccountId>95</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Daniel Alejandro Angel Fuertes</DisplayName>
+        <AccountId>55</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Jeniffer Liliam Mendoza Espinosa</DisplayName>
+        <AccountId>97</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Kevin Cohen Solano</DisplayName>
+        <AccountId>93</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Cesar Luis Moreno Gonzalez</DisplayName>
+        <AccountId>96</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Jose Cristobal Arroyo Castellanos</DisplayName>
+        <AccountId>54</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97C5E1E0-C817-4769-9D2D-1DC296B681FA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8DF3742-38F2-4B99-B335-CC4F04ED9F45}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="164883f8-7691-4ecf-b54a-664c0d0edefe"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="85e30bcc-d76c-4413-8e4d-2dce22fb0743"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5760,9 +5836,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8DF3742-38F2-4B99-B335-CC4F04ED9F45}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97C5E1E0-C817-4769-9D2D-1DC296B681FA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="164883f8-7691-4ecf-b54a-664c0d0edefe"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="85e30bcc-d76c-4413-8e4d-2dce22fb0743"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>